<commit_message>
Changing the freeze panes
</commit_message>
<xml_diff>
--- a/refs/litreview/full_review_guide.xlsx
+++ b/refs/litreview/full_review_guide.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/decsens/refs/litreview/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12960" windowWidth="40840" windowHeight="16600"/>
+    <workbookView xWindow="18600" yWindow="5640" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="decsens review" sheetId="1" r:id="rId1"/>
     <sheet name="meta" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -468,7 +466,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -581,7 +579,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -633,7 +631,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -827,7 +825,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -838,14 +836,16 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="A25:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
@@ -853,7 +853,7 @@
     <col min="10" max="10" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +885,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -911,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="48">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -943,7 +943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="144">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -975,7 +975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="112">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="80">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="112">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="64">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="32">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="80">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="64">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="64">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="192">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="96">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="48">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="176">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="144">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="32">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="64">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="64">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="32">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="48">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="96">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -1748,6 +1748,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1759,13 +1764,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="46.5" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -1776,7 +1781,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1792,7 +1797,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1800,7 +1805,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1808,7 +1813,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1816,7 +1821,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1824,7 +1829,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -1834,5 +1839,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated citations for decsens
</commit_message>
<xml_diff>
--- a/refs/litreview/full_review_guide.xlsx
+++ b/refs/litreview/full_review_guide.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/decsens/refs/litreview/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="5640" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="23100" yWindow="4440" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="decsens review" sheetId="1" r:id="rId1"/>
     <sheet name="meta" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -274,9 +279,6 @@
     <t>4 European species</t>
   </si>
   <si>
-    <t>Wang2014</t>
-  </si>
-  <si>
     <t>PEP sps</t>
   </si>
   <si>
@@ -298,9 +300,6 @@
     <t>Wang2017</t>
   </si>
   <si>
-    <t>Wenden</t>
-  </si>
-  <si>
     <t>Quercus and Fagus clones</t>
   </si>
   <si>
@@ -461,12 +460,18 @@
   </si>
   <si>
     <t>3,6</t>
+  </si>
+  <si>
+    <t>Wang2016gcb</t>
+  </si>
+  <si>
+    <t>Wenden2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -825,7 +830,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -836,13 +841,13 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="A25:J25"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
@@ -853,7 +858,7 @@
     <col min="10" max="10" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,10 +887,10 @@
         <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -911,7 +916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="48">
+    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -943,7 +948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="144">
+    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -975,7 +980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="112">
+    <row r="5" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="80">
+    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1068,7 +1073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="112">
+    <row r="8" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1100,7 +1105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="64">
+    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1129,10 +1134,10 @@
         <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="32">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1164,7 +1169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="80">
+    <row r="11" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1190,13 +1195,13 @@
         <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="64">
+    <row r="12" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1225,7 +1230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="64">
+    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1254,7 +1259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1277,7 +1282,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="192">
+    <row r="15" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1309,7 +1314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="96">
+    <row r="16" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1335,18 +1340,18 @@
         <v>4</v>
       </c>
       <c r="J16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="48">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -1358,10 +1363,10 @@
         <v>15</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
         <v>85</v>
-      </c>
-      <c r="H17" t="s">
-        <v>86</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1370,15 +1375,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="176">
+    <row r="18" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -1390,7 +1395,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I18" t="s">
         <v>80</v>
@@ -1399,15 +1404,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="144">
+    <row r="19" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -1419,27 +1424,27 @@
         <v>40</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" t="s">
+        <v>86</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>93</v>
       </c>
-      <c r="H19" t="s">
+      <c r="B20" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
         <v>95</v>
-      </c>
-      <c r="B20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
@@ -1451,7 +1456,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I20">
         <v>3</v>
@@ -1460,15 +1465,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="32">
+    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" t="s">
-        <v>100</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -1477,36 +1482,36 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
         <v>103</v>
       </c>
-      <c r="J21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="64">
-      <c r="A22" t="s">
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="I22" t="s">
         <v>80</v>
@@ -1515,15 +1520,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1541,27 +1546,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="64">
+    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
         <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I24">
         <v>6</v>
@@ -1570,15 +1575,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="32">
+    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
         <v>113</v>
-      </c>
-      <c r="B25" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25" t="s">
-        <v>115</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -1590,10 +1595,10 @@
         <v>15</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1602,41 +1607,41 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" t="s">
         <v>117</v>
       </c>
-      <c r="B26" t="s">
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D26" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="I26" t="s">
         <v>79</v>
       </c>
       <c r="J26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="48">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
         <v>30</v>
@@ -1648,27 +1653,27 @@
         <v>15</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" t="s">
         <v>130</v>
       </c>
-      <c r="J27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="96">
-      <c r="A28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" t="s">
-        <v>132</v>
-      </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
@@ -1680,25 +1685,25 @@
         <v>15</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" t="s">
         <v>132</v>
-      </c>
-      <c r="C29" t="s">
-        <v>134</v>
       </c>
       <c r="D29" t="s">
         <v>55</v>
@@ -1710,36 +1715,36 @@
         <v>15</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B30" t="s">
+      <c r="I30" t="s">
         <v>143</v>
-      </c>
-      <c r="C30" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I30" t="s">
-        <v>145</v>
       </c>
       <c r="J30" t="s">
         <v>10</v>
@@ -1764,24 +1769,24 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="46.5" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1789,7 +1794,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1813,7 +1818,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1821,15 +1826,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
added preseaon information for phenology studies in full_review_guide spread sheet
</commit_message>
<xml_diff>
--- a/refs/litreview/full_review_guide.xlsx
+++ b/refs/litreview/full_review_guide.xlsx
@@ -1,34 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/decsens/refs/litreview/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27226"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23100" yWindow="4440" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="4460" yWindow="3740" windowWidth="37060" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="decsens review" sheetId="1" r:id="rId1"/>
     <sheet name="meta" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="159">
   <si>
     <t>studyID</t>
   </si>
@@ -466,13 +461,52 @@
   </si>
   <si>
     <t>Wenden2019</t>
+  </si>
+  <si>
+    <t>preseason</t>
+  </si>
+  <si>
+    <t>no mention</t>
+  </si>
+  <si>
+    <t>Nov1-April 30</t>
+  </si>
+  <si>
+    <t>The optimal preseason for RP (relevant preseason) was defined as the period (at 15-day intervals) before the mean leaf unfolding date for which the Pearson correlation coefficient between leaf unfolding and air temperature was highest. The core algorithm for these models was ordinary least squares.</t>
+  </si>
+  <si>
+    <t>Similarly to previous studies (Matsumoto et al. 2003; Dai et al. 2013), we estimated the optimum preseason (OP) that affects the phenophase most significantly for each species. First, we calculated the mean occurrence of LUD over the study period for each species, which was defined as the end date of OP (EP). We then calculated the start date of the OP (BP) by moving the date from EP-120 (120 days before EP) to EP-1 (the day before EP) in steps of 15 days. PearsonÕs correlation analysis was performed to compare the series of data from each year and the mean temperature during each [BP, EP] period. The [BP, EP] period showing the correlation coefficient (R) with the highest absolute value was taken as the OP. (Dan's note 30-90 days was the OP for most)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> November to the mean date of leaf unfolding (MSOS)</t>
+  </si>
+  <si>
+    <t>I think not applicable</t>
+  </si>
+  <si>
+    <t>The phenology-based three-season division (no autumn) was determined from the partial correlation of the SOS to the climate of the individual month before the average SOS (Suppl. Material Fig. S1) and differs from a calendar-based four-season division.</t>
+  </si>
+  <si>
+    <t>to August of the year of tree-ring formation Ð</t>
+  </si>
+  <si>
+    <t>tarting from June of the previous year to August of the year of tree-ring formation</t>
+  </si>
+  <si>
+    <t>specifically varied (one of the main points of this study)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The preseason at each station was defined as the period (with 5 day steps) before the mean FBD for which the Spearman's rank correlation coefficient between FBD and mean temperature was highest during 1963Ð2013 (H. Wang, Zhong, et al., 2017).</t>
+  </si>
+  <si>
+    <t>Here preseason temperature is defined as the mean temperature for the two months with the later month containing the 27-year average (1982Ð2008) of spring phenological date for each pixel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,6 +528,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -512,10 +562,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -524,8 +580,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -830,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -838,16 +906,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
@@ -856,9 +924,10 @@
     <col min="7" max="7" width="50" customWidth="1"/>
     <col min="8" max="8" width="41.5" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,8 +958,11 @@
       <c r="J1" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -915,8 +987,11 @@
       <c r="J2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -947,8 +1022,11 @@
       <c r="J3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="180">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -979,8 +1057,11 @@
       <c r="J4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="K4" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="409">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1011,8 +1092,11 @@
       <c r="J5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1040,8 +1124,11 @@
       <c r="J6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="K6" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="80">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1072,8 +1159,11 @@
       <c r="J7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="150">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1104,8 +1194,11 @@
       <c r="J8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="K8" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1136,8 +1229,11 @@
       <c r="J9" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="K9" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1168,8 +1264,11 @@
       <c r="J10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="K10" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="75">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1200,8 +1299,11 @@
       <c r="J11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="K11" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="64">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1230,7 +1332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="64">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1259,7 +1361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1282,7 +1384,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="192">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1314,7 +1416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="96">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1343,7 +1445,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="48">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -1375,7 +1477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="165">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1403,8 +1505,11 @@
       <c r="J18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+      <c r="K18" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="120">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -1436,7 +1541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1465,7 +1570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -1491,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="60">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -1520,7 +1625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -1546,7 +1651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="64">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1574,8 +1679,11 @@
       <c r="J24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="150">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -1606,8 +1714,11 @@
       <c r="J25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -1633,7 +1744,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="48">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -1665,7 +1776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="96">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -1695,7 +1806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -1724,7 +1835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -1752,7 +1863,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1769,13 +1880,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="46.5" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -1786,7 +1897,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1794,7 +1905,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1802,7 +1913,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1810,7 +1921,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1818,7 +1929,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1826,7 +1937,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1834,7 +1945,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>80</v>
       </c>

</xml_diff>